<commit_message>
[Feat] Cambiar hora en Curva de Tolerancia Excel y Datos en formato pdf Captura
</commit_message>
<xml_diff>
--- a/Service.MedicalRecord/wwwroot/layout/excel/deliverResults/CurvaTolerancia.xlsx
+++ b/Service.MedicalRecord/wwwroot/layout/excel/deliverResults/CurvaTolerancia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JuanDanielGonzalezAl\Documents\Projects\API\Service.MedicalRecord\wwwroot\layout\excel\deliverResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC09806-9DA8-40F8-9103-4A2AEEB3F000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30BEC506-AE8C-41CA-B3E1-3311545B2E11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{ABA354A7-6530-45F0-99BA-AEAF3E0C68E7}"/>
   </bookViews>
@@ -42,10 +42,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>LABORATORIO ALFONSO RAMOS S.A. DE C.V.</t>
-  </si>
-  <si>
-    <t>TIEMPO DE GLUCEMA OBTENIDA EN LA PRUEBA DE TOLERANCIA A GLUCOSA CON DOSIS ÚNICA 
-Y OBSERVACIONES DE DOS HORAS</t>
   </si>
   <si>
     <t>PACIENTE:</t>
@@ -85,6 +81,10 @@
   </si>
   <si>
     <t>{{item.Estudio}}</t>
+  </si>
+  <si>
+    <t>TIEMPO DE GLUCEMA OBTENIDA EN LA PRUEBA DE TOLERANCIA A GLUCOSA CON DOSIS ÚNICA 
+Y OBSERVACIONES DE {{Tiempo}}</t>
   </si>
 </sst>
 </file>
@@ -1437,10 +1437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4937A528-F84F-4530-896A-BD7902E0DE2F}">
-  <dimension ref="B2:K41"/>
+  <dimension ref="B2:N41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1452,7 +1452,7 @@
     <col min="8" max="8" width="37.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
@@ -1465,7 +1465,7 @@
       <c r="I2" s="9"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
@@ -1476,12 +1476,15 @@
       <c r="I3" s="9"/>
       <c r="J3" s="2"/>
     </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="N16" s="7"/>
+    </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="K20" s="7"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C25" s="11"/>
       <c r="D25" s="11"/>
@@ -1503,53 +1506,53 @@
     </row>
     <row r="28" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C29" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B35" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G28" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H28" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B29" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B31" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D34" s="3" t="s">
+      <c r="D35" s="1" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B35" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>